<commit_message>
just added some more documentations
</commit_message>
<xml_diff>
--- a/documentations/product plan.xlsx
+++ b/documentations/product plan.xlsx
@@ -1,20 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Auralis2.0\Auralis\documentations\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE510046-9F37-4E9A-978D-963223A66D5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="1. Product Overview" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="2. Product Backlog" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="3. Roadmap" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="4. Retrospective" sheetId="4" r:id="rId7"/>
+    <sheet name="1. Product Overview" sheetId="1" r:id="rId1"/>
+    <sheet name="2. Product Backlog" sheetId="2" r:id="rId2"/>
+    <sheet name="3. Roadmap" sheetId="3" r:id="rId3"/>
+    <sheet name="4. Retrospective" sheetId="4" r:id="rId4"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="163">
   <si>
     <t>Item</t>
   </si>
@@ -454,9 +463,6 @@
     <t>Backend model integration</t>
   </si>
   <si>
-    <t>on track</t>
-  </si>
-  <si>
     <t>v1.0</t>
   </si>
   <si>
@@ -470,9 +476,6 @@
   </si>
   <si>
     <t>v1.1</t>
-  </si>
-  <si>
-    <t>Analytics export, Notification system</t>
   </si>
   <si>
     <t>UI design system</t>
@@ -480,16 +483,16 @@
   <si>
     <r>
       <rPr>
+        <b/>
+        <sz val="11"/>
         <rFont val="Calibri"/>
-        <b/>
-        <sz val="11.0"/>
       </rPr>
       <t>Note:</t>
     </r>
     <r>
       <rPr>
+        <sz val="11"/>
         <rFont val="Calibri"/>
-        <sz val="11.0"/>
       </rPr>
       <t xml:space="preserve"> This is for the team to learn and improve. I have taught you in the class on Nov 4, 2025.</t>
     </r>
@@ -520,30 +523,33 @@
   </si>
   <si>
     <t>Test Lead</t>
+  </si>
+  <si>
+    <t>Analytics export-report generation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="8.0"/>
+      <sz val="8"/>
       <color rgb="FF0A0A0A"/>
       <name val="Arial"/>
     </font>
@@ -553,11 +559,17 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -571,62 +583,51 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="16" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
     <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -784,7 +785,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln cap="flat" cmpd="sng" w="9525" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -793,13 +794,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln cap="flat" cmpd="sng" w="25400" algn="ctr">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln cap="flat" cmpd="sng" w="38100" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -809,7 +810,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" rotWithShape="0" dir="5400000" dist="20000">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -818,7 +819,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" rotWithShape="0" dir="5400000" dist="23000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -827,7 +828,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" rotWithShape="0" dir="5400000" dist="23000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -837,12 +838,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -873,7 +874,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -892,32 +893,31 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B100"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="31.0"/>
-    <col customWidth="1" min="2" max="2" width="55.0"/>
-    <col customWidth="1" min="3" max="6" width="9.0"/>
+    <col min="1" max="1" width="31" customWidth="1"/>
+    <col min="2" max="2" width="55" customWidth="1"/>
+    <col min="3" max="6" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
+    <row r="1" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -925,7 +925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="14.25" customHeight="1">
+    <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -933,7 +933,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" ht="14.25" customHeight="1">
+    <row r="3" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -941,7 +941,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" ht="14.25" customHeight="1">
+    <row r="4" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -949,7 +949,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" ht="14.25" customHeight="1">
+    <row r="5" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -957,132 +957,130 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" ht="14.25" customHeight="1"/>
-    <row r="7" ht="14.25" customHeight="1"/>
-    <row r="8" ht="14.25" customHeight="1"/>
-    <row r="9" ht="14.25" customHeight="1"/>
-    <row r="10" ht="14.25" customHeight="1"/>
-    <row r="11" ht="14.25" customHeight="1"/>
-    <row r="12" ht="14.25" customHeight="1"/>
-    <row r="13" ht="14.25" customHeight="1"/>
-    <row r="14" ht="14.25" customHeight="1"/>
-    <row r="15" ht="14.25" customHeight="1"/>
-    <row r="16" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
-    <row r="49" ht="14.25" customHeight="1"/>
-    <row r="50" ht="14.25" customHeight="1"/>
-    <row r="51" ht="14.25" customHeight="1"/>
-    <row r="52" ht="14.25" customHeight="1"/>
-    <row r="53" ht="14.25" customHeight="1"/>
-    <row r="54" ht="14.25" customHeight="1"/>
-    <row r="55" ht="14.25" customHeight="1"/>
-    <row r="56" ht="14.25" customHeight="1"/>
-    <row r="57" ht="14.25" customHeight="1"/>
-    <row r="58" ht="14.25" customHeight="1"/>
-    <row r="59" ht="14.25" customHeight="1"/>
-    <row r="60" ht="14.25" customHeight="1"/>
-    <row r="61" ht="14.25" customHeight="1"/>
-    <row r="62" ht="14.25" customHeight="1"/>
-    <row r="63" ht="14.25" customHeight="1"/>
-    <row r="64" ht="14.25" customHeight="1"/>
-    <row r="65" ht="14.25" customHeight="1"/>
-    <row r="66" ht="14.25" customHeight="1"/>
-    <row r="67" ht="14.25" customHeight="1"/>
-    <row r="68" ht="14.25" customHeight="1"/>
-    <row r="69" ht="14.25" customHeight="1"/>
-    <row r="70" ht="14.25" customHeight="1"/>
-    <row r="71" ht="14.25" customHeight="1"/>
-    <row r="72" ht="14.25" customHeight="1"/>
-    <row r="73" ht="14.25" customHeight="1"/>
-    <row r="74" ht="14.25" customHeight="1"/>
-    <row r="75" ht="14.25" customHeight="1"/>
-    <row r="76" ht="14.25" customHeight="1"/>
-    <row r="77" ht="14.25" customHeight="1"/>
-    <row r="78" ht="14.25" customHeight="1"/>
-    <row r="79" ht="14.25" customHeight="1"/>
-    <row r="80" ht="14.25" customHeight="1"/>
-    <row r="81" ht="14.25" customHeight="1"/>
-    <row r="82" ht="14.25" customHeight="1"/>
-    <row r="83" ht="14.25" customHeight="1"/>
-    <row r="84" ht="14.25" customHeight="1"/>
-    <row r="85" ht="14.25" customHeight="1"/>
-    <row r="86" ht="14.25" customHeight="1"/>
-    <row r="87" ht="14.25" customHeight="1"/>
-    <row r="88" ht="14.25" customHeight="1"/>
-    <row r="89" ht="14.25" customHeight="1"/>
-    <row r="90" ht="14.25" customHeight="1"/>
-    <row r="91" ht="14.25" customHeight="1"/>
-    <row r="92" ht="14.25" customHeight="1"/>
-    <row r="93" ht="14.25" customHeight="1"/>
-    <row r="94" ht="14.25" customHeight="1"/>
-    <row r="95" ht="14.25" customHeight="1"/>
-    <row r="96" ht="14.25" customHeight="1"/>
-    <row r="97" ht="14.25" customHeight="1"/>
-    <row r="98" ht="14.25" customHeight="1"/>
-    <row r="99" ht="14.25" customHeight="1"/>
-    <row r="100" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="9.0"/>
-    <col customWidth="1" min="2" max="2" width="28.0"/>
-    <col customWidth="1" min="3" max="3" width="11.71"/>
-    <col customWidth="1" min="4" max="4" width="73.29"/>
-    <col customWidth="1" min="5" max="5" width="21.43"/>
-    <col customWidth="1" min="6" max="6" width="16.57"/>
-    <col customWidth="1" min="7" max="8" width="11.43"/>
-    <col customWidth="1" min="9" max="9" width="22.43"/>
-    <col customWidth="1" min="10" max="10" width="22.71"/>
-    <col customWidth="1" min="11" max="11" width="10.57"/>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="2" max="2" width="28" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="73.28515625" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="7" max="8" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" customWidth="1"/>
+    <col min="10" max="10" width="22.7109375" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
+    <row r="1" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1117,7 +1115,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" ht="14.25" customHeight="1">
+    <row r="2" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>21</v>
@@ -1146,7 +1144,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" ht="14.25" customHeight="1">
+    <row r="3" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
@@ -1179,7 +1177,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" ht="14.25" customHeight="1">
+    <row r="4" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>34</v>
       </c>
@@ -1212,7 +1210,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" ht="14.25" customHeight="1">
+    <row r="5" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>43</v>
       </c>
@@ -1243,7 +1241,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" ht="14.25" customHeight="1">
+    <row r="6" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>49</v>
       </c>
@@ -1276,7 +1274,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" ht="14.25" customHeight="1">
+    <row r="7" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>54</v>
       </c>
@@ -1309,7 +1307,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" ht="14.25" customHeight="1">
+    <row r="8" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1322,7 +1320,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" ht="14.25" customHeight="1">
+    <row r="9" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>59</v>
       </c>
@@ -1355,7 +1353,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" ht="14.25" customHeight="1">
+    <row r="10" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>66</v>
       </c>
@@ -1388,7 +1386,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" ht="14.25" customHeight="1">
+    <row r="11" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>71</v>
       </c>
@@ -1421,7 +1419,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" ht="14.25" customHeight="1">
+    <row r="12" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>78</v>
       </c>
@@ -1454,7 +1452,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" ht="14.25" customHeight="1">
+    <row r="13" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>84</v>
       </c>
@@ -1487,7 +1485,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" ht="14.25" customHeight="1">
+    <row r="14" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>90</v>
       </c>
@@ -1520,7 +1518,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" ht="14.25" customHeight="1">
+    <row r="15" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1533,7 +1531,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" ht="14.25" customHeight="1">
+    <row r="16" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>97</v>
       </c>
@@ -1566,7 +1564,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" ht="14.25" customHeight="1">
+    <row r="17" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>103</v>
       </c>
@@ -1597,7 +1595,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" ht="14.25" customHeight="1">
+    <row r="18" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>107</v>
       </c>
@@ -1626,8 +1624,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1">
+    <row r="19" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>111</v>
       </c>
@@ -1637,7 +1635,7 @@
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" ht="14.25" customHeight="1">
+    <row r="21" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>29</v>
       </c>
@@ -1646,7 +1644,7 @@
       </c>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" ht="14.25" customHeight="1">
+    <row r="22" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>64</v>
       </c>
@@ -1655,7 +1653,7 @@
       </c>
       <c r="E22" s="6"/>
     </row>
-    <row r="23" ht="14.25" customHeight="1">
+    <row r="23" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>83</v>
       </c>
@@ -1664,7 +1662,7 @@
       </c>
       <c r="E23" s="5"/>
     </row>
-    <row r="24" ht="14.25" customHeight="1">
+    <row r="24" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>116</v>
       </c>
@@ -1673,13 +1671,13 @@
       </c>
       <c r="E24" s="5"/>
     </row>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1">
+    <row r="25" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="27" ht="14.25" customHeight="1">
+    <row r="27" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>118</v>
       </c>
@@ -1687,7 +1685,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="28" ht="14.25" customHeight="1">
+    <row r="28" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>120</v>
       </c>
@@ -1695,109 +1693,107 @@
         <v>121</v>
       </c>
     </row>
-    <row r="29" ht="14.25" customHeight="1">
+    <row r="29" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
-    <row r="49" ht="14.25" customHeight="1"/>
-    <row r="50" ht="14.25" customHeight="1"/>
-    <row r="51" ht="14.25" customHeight="1"/>
-    <row r="52" ht="14.25" customHeight="1"/>
-    <row r="53" ht="14.25" customHeight="1"/>
-    <row r="54" ht="14.25" customHeight="1"/>
-    <row r="55" ht="14.25" customHeight="1"/>
-    <row r="56" ht="14.25" customHeight="1"/>
-    <row r="57" ht="14.25" customHeight="1"/>
-    <row r="58" ht="14.25" customHeight="1"/>
-    <row r="59" ht="14.25" customHeight="1"/>
-    <row r="60" ht="14.25" customHeight="1"/>
-    <row r="61" ht="14.25" customHeight="1"/>
-    <row r="62" ht="14.25" customHeight="1"/>
-    <row r="63" ht="14.25" customHeight="1"/>
-    <row r="64" ht="14.25" customHeight="1"/>
-    <row r="65" ht="14.25" customHeight="1"/>
-    <row r="66" ht="14.25" customHeight="1"/>
-    <row r="67" ht="14.25" customHeight="1"/>
-    <row r="68" ht="14.25" customHeight="1"/>
-    <row r="69" ht="14.25" customHeight="1"/>
-    <row r="70" ht="14.25" customHeight="1"/>
-    <row r="71" ht="14.25" customHeight="1"/>
-    <row r="72" ht="14.25" customHeight="1"/>
-    <row r="73" ht="14.25" customHeight="1"/>
-    <row r="74" ht="14.25" customHeight="1"/>
-    <row r="75" ht="14.25" customHeight="1"/>
-    <row r="76" ht="14.25" customHeight="1"/>
-    <row r="77" ht="14.25" customHeight="1"/>
-    <row r="78" ht="14.25" customHeight="1"/>
-    <row r="79" ht="14.25" customHeight="1"/>
-    <row r="80" ht="14.25" customHeight="1"/>
-    <row r="81" ht="14.25" customHeight="1"/>
-    <row r="82" ht="14.25" customHeight="1"/>
-    <row r="83" ht="14.25" customHeight="1"/>
-    <row r="84" ht="14.25" customHeight="1"/>
-    <row r="85" ht="14.25" customHeight="1"/>
-    <row r="86" ht="14.25" customHeight="1"/>
-    <row r="87" ht="14.25" customHeight="1"/>
-    <row r="88" ht="14.25" customHeight="1"/>
-    <row r="89" ht="14.25" customHeight="1"/>
-    <row r="90" ht="14.25" customHeight="1"/>
-    <row r="91" ht="14.25" customHeight="1"/>
-    <row r="92" ht="14.25" customHeight="1"/>
-    <row r="93" ht="14.25" customHeight="1"/>
-    <row r="94" ht="14.25" customHeight="1"/>
-    <row r="95" ht="14.25" customHeight="1"/>
-    <row r="96" ht="14.25" customHeight="1"/>
-    <row r="97" ht="14.25" customHeight="1"/>
-    <row r="98" ht="14.25" customHeight="1"/>
-    <row r="99" ht="14.25" customHeight="1"/>
-    <row r="100" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="7.14"/>
-    <col customWidth="1" min="2" max="2" width="10.57"/>
-    <col customWidth="1" min="3" max="3" width="44.0"/>
-    <col customWidth="1" min="4" max="4" width="21.29"/>
-    <col customWidth="1" min="5" max="5" width="17.14"/>
-    <col customWidth="1" min="6" max="6" width="9.0"/>
+    <col min="1" max="1" width="7.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="44" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="6" max="6" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>123</v>
       </c>
@@ -1814,7 +1810,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" ht="14.25" customHeight="1">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
@@ -1823,12 +1819,12 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" ht="14.25" customHeight="1">
+    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>129</v>
       </c>
       <c r="B3" s="7">
-        <v>45976.0</v>
+        <v>45976</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>130</v>
@@ -1840,12 +1836,12 @@
         <v>132</v>
       </c>
     </row>
-    <row r="4" ht="14.25" customHeight="1">
+    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>133</v>
       </c>
       <c r="B4" s="7">
-        <v>45983.0</v>
+        <v>45983</v>
       </c>
       <c r="C4" t="s">
         <v>134</v>
@@ -1857,12 +1853,12 @@
         <v>132</v>
       </c>
     </row>
-    <row r="5" ht="14.25" customHeight="1">
+    <row r="5" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>136</v>
       </c>
       <c r="B5" s="7">
-        <v>45990.0</v>
+        <v>45990</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>137</v>
@@ -1874,12 +1870,12 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" ht="14.25" customHeight="1">
+    <row r="6" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>139</v>
       </c>
       <c r="B6" s="7">
-        <v>45997.0</v>
+        <v>45997</v>
       </c>
       <c r="C6" t="s">
         <v>140</v>
@@ -1887,16 +1883,16 @@
       <c r="D6" t="s">
         <v>141</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="7" ht="14.25" customHeight="1">
+    <row r="7" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>143</v>
       </c>
       <c r="B7" s="7">
-        <v>46004.0</v>
+        <v>46004</v>
       </c>
       <c r="C7" t="s">
         <v>144</v>
@@ -1904,341 +1900,335 @@
       <c r="D7" t="s">
         <v>145</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="2" t="s">
+      <c r="B8" s="7">
+        <v>46011</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D8" t="s">
+        <v>148</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B9" s="7">
+        <v>46018</v>
+      </c>
+      <c r="C9" t="s">
         <v>147</v>
       </c>
-      <c r="B8" s="7">
-        <v>46011.0</v>
-      </c>
-      <c r="C8" t="s">
-        <v>148</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
+        <v>151</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B9" s="7">
-        <v>46018.0</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="D9" t="s">
-        <v>153</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="10" ht="14.25" customHeight="1">
+    </row>
+    <row r="10" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" ht="14.25" customHeight="1"/>
-    <row r="12" ht="14.25" customHeight="1"/>
-    <row r="13" ht="14.25" customHeight="1"/>
-    <row r="14" ht="14.25" customHeight="1"/>
-    <row r="15" ht="14.25" customHeight="1"/>
-    <row r="16" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
-    <row r="49" ht="14.25" customHeight="1"/>
-    <row r="50" ht="14.25" customHeight="1"/>
-    <row r="51" ht="14.25" customHeight="1"/>
-    <row r="52" ht="14.25" customHeight="1"/>
-    <row r="53" ht="14.25" customHeight="1"/>
-    <row r="54" ht="14.25" customHeight="1"/>
-    <row r="55" ht="14.25" customHeight="1"/>
-    <row r="56" ht="14.25" customHeight="1"/>
-    <row r="57" ht="14.25" customHeight="1"/>
-    <row r="58" ht="14.25" customHeight="1"/>
-    <row r="59" ht="14.25" customHeight="1"/>
-    <row r="60" ht="14.25" customHeight="1"/>
-    <row r="61" ht="14.25" customHeight="1"/>
-    <row r="62" ht="14.25" customHeight="1"/>
-    <row r="63" ht="14.25" customHeight="1"/>
-    <row r="64" ht="14.25" customHeight="1"/>
-    <row r="65" ht="14.25" customHeight="1"/>
-    <row r="66" ht="14.25" customHeight="1"/>
-    <row r="67" ht="14.25" customHeight="1"/>
-    <row r="68" ht="14.25" customHeight="1"/>
-    <row r="69" ht="14.25" customHeight="1"/>
-    <row r="70" ht="14.25" customHeight="1"/>
-    <row r="71" ht="14.25" customHeight="1"/>
-    <row r="72" ht="14.25" customHeight="1"/>
-    <row r="73" ht="14.25" customHeight="1"/>
-    <row r="74" ht="14.25" customHeight="1"/>
-    <row r="75" ht="14.25" customHeight="1"/>
-    <row r="76" ht="14.25" customHeight="1"/>
-    <row r="77" ht="14.25" customHeight="1"/>
-    <row r="78" ht="14.25" customHeight="1"/>
-    <row r="79" ht="14.25" customHeight="1"/>
-    <row r="80" ht="14.25" customHeight="1"/>
-    <row r="81" ht="14.25" customHeight="1"/>
-    <row r="82" ht="14.25" customHeight="1"/>
-    <row r="83" ht="14.25" customHeight="1"/>
-    <row r="84" ht="14.25" customHeight="1"/>
-    <row r="85" ht="14.25" customHeight="1"/>
-    <row r="86" ht="14.25" customHeight="1"/>
-    <row r="87" ht="14.25" customHeight="1"/>
-    <row r="88" ht="14.25" customHeight="1"/>
-    <row r="89" ht="14.25" customHeight="1"/>
-    <row r="90" ht="14.25" customHeight="1"/>
-    <row r="91" ht="14.25" customHeight="1"/>
-    <row r="92" ht="14.25" customHeight="1"/>
-    <row r="93" ht="14.25" customHeight="1"/>
-    <row r="94" ht="14.25" customHeight="1"/>
-    <row r="95" ht="14.25" customHeight="1"/>
-    <row r="96" ht="14.25" customHeight="1"/>
-    <row r="97" ht="14.25" customHeight="1"/>
-    <row r="98" ht="14.25" customHeight="1"/>
-    <row r="99" ht="14.25" customHeight="1"/>
-    <row r="100" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:D100"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="25.71"/>
-    <col customWidth="1" min="2" max="2" width="27.71"/>
-    <col customWidth="1" min="3" max="3" width="31.57"/>
-    <col customWidth="1" min="4" max="4" width="9.43"/>
-    <col customWidth="1" min="5" max="6" width="9.0"/>
+    <col min="1" max="1" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="3" max="3" width="31.5703125" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
+    <col min="5" max="6" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1"/>
-    <row r="2" ht="14.25" customHeight="1">
+    <row r="1" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" t="s">
+      <c r="B5" s="1" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="4" ht="14.25" customHeight="1"/>
-    <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>158</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" ht="14.25" customHeight="1">
+    <row r="6" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="8" ht="14.25" customHeight="1">
+    </row>
+    <row r="8" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" ht="14.25" customHeight="1">
+    <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" ht="14.25" customHeight="1">
+    <row r="10" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" ht="14.25" customHeight="1">
+    <row r="11" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" ht="14.25" customHeight="1">
+    <row r="12" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" ht="14.25" customHeight="1">
+    <row r="13" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" ht="14.25" customHeight="1"/>
-    <row r="15" ht="14.25" customHeight="1"/>
-    <row r="16" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
-    <row r="49" ht="14.25" customHeight="1"/>
-    <row r="50" ht="14.25" customHeight="1"/>
-    <row r="51" ht="14.25" customHeight="1"/>
-    <row r="52" ht="14.25" customHeight="1"/>
-    <row r="53" ht="14.25" customHeight="1"/>
-    <row r="54" ht="14.25" customHeight="1"/>
-    <row r="55" ht="14.25" customHeight="1"/>
-    <row r="56" ht="14.25" customHeight="1"/>
-    <row r="57" ht="14.25" customHeight="1"/>
-    <row r="58" ht="14.25" customHeight="1"/>
-    <row r="59" ht="14.25" customHeight="1"/>
-    <row r="60" ht="14.25" customHeight="1"/>
-    <row r="61" ht="14.25" customHeight="1"/>
-    <row r="62" ht="14.25" customHeight="1"/>
-    <row r="63" ht="14.25" customHeight="1"/>
-    <row r="64" ht="14.25" customHeight="1"/>
-    <row r="65" ht="14.25" customHeight="1"/>
-    <row r="66" ht="14.25" customHeight="1"/>
-    <row r="67" ht="14.25" customHeight="1"/>
-    <row r="68" ht="14.25" customHeight="1"/>
-    <row r="69" ht="14.25" customHeight="1"/>
-    <row r="70" ht="14.25" customHeight="1"/>
-    <row r="71" ht="14.25" customHeight="1"/>
-    <row r="72" ht="14.25" customHeight="1"/>
-    <row r="73" ht="14.25" customHeight="1"/>
-    <row r="74" ht="14.25" customHeight="1"/>
-    <row r="75" ht="14.25" customHeight="1"/>
-    <row r="76" ht="14.25" customHeight="1"/>
-    <row r="77" ht="14.25" customHeight="1"/>
-    <row r="78" ht="14.25" customHeight="1"/>
-    <row r="79" ht="14.25" customHeight="1"/>
-    <row r="80" ht="14.25" customHeight="1"/>
-    <row r="81" ht="14.25" customHeight="1"/>
-    <row r="82" ht="14.25" customHeight="1"/>
-    <row r="83" ht="14.25" customHeight="1"/>
-    <row r="84" ht="14.25" customHeight="1"/>
-    <row r="85" ht="14.25" customHeight="1"/>
-    <row r="86" ht="14.25" customHeight="1"/>
-    <row r="87" ht="14.25" customHeight="1"/>
-    <row r="88" ht="14.25" customHeight="1"/>
-    <row r="89" ht="14.25" customHeight="1"/>
-    <row r="90" ht="14.25" customHeight="1"/>
-    <row r="91" ht="14.25" customHeight="1"/>
-    <row r="92" ht="14.25" customHeight="1"/>
-    <row r="93" ht="14.25" customHeight="1"/>
-    <row r="94" ht="14.25" customHeight="1"/>
-    <row r="95" ht="14.25" customHeight="1"/>
-    <row r="96" ht="14.25" customHeight="1"/>
-    <row r="97" ht="14.25" customHeight="1"/>
-    <row r="98" ht="14.25" customHeight="1"/>
-    <row r="99" ht="14.25" customHeight="1"/>
-    <row r="100" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>